<commit_message>
correction des tests suite a la revision de Boivin
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Nicolas</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>Note sur 100</t>
+  </si>
+  <si>
+    <t>Somme</t>
   </si>
 </sst>
 </file>
@@ -284,6 +287,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -609,18 +617,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="8" width="10.83203125" style="1"/>
+    <col min="2" max="8" width="10.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>42</v>
       </c>
@@ -643,7 +651,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>35</v>
       </c>
@@ -665,8 +673,11 @@
       <c r="H2" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="J2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -691,8 +702,12 @@
       <c r="H3" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="J3">
+        <f>SUM(B3:G3)</f>
+        <v>14.64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -717,8 +732,16 @@
       <c r="H4" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="J4">
+        <f t="shared" ref="J4:J37" si="0">SUM(B4:G4)</f>
+        <v>14.5</v>
+      </c>
+      <c r="L4">
+        <f>CORREL(J3:J37,H3:H37)</f>
+        <v>0.27181211883882611</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -743,8 +766,12 @@
       <c r="H5" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>9.5399999999999991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -769,8 +796,12 @@
       <c r="H6" s="1">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>13.29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -795,8 +826,12 @@
       <c r="H7" s="1">
         <v>62</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>13.309999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -821,8 +856,12 @@
       <c r="H8" s="1">
         <v>68</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>13.579999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -847,8 +886,12 @@
       <c r="H9" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>14.26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -873,8 +916,12 @@
       <c r="H10" s="1">
         <v>95</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>12.690000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -888,7 +935,7 @@
         <v>0.38</v>
       </c>
       <c r="E11" s="1">
-        <v>3.53</v>
+        <v>0</v>
       </c>
       <c r="F11" s="1">
         <v>1.81</v>
@@ -899,8 +946,12 @@
       <c r="H11" s="1">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>9.4500000000000011</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -925,8 +976,12 @@
       <c r="H12" s="1">
         <v>96</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>15.49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -951,8 +1006,12 @@
       <c r="H13" s="1">
         <v>69</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>14.889999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -977,8 +1036,12 @@
       <c r="H14" s="1">
         <v>91</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>14.74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1003,8 +1066,12 @@
       <c r="H15" s="1">
         <v>73</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>16.049999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1029,8 +1096,12 @@
       <c r="H16" s="1">
         <v>69</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>19.07</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1044,7 +1115,7 @@
         <v>2.6</v>
       </c>
       <c r="E17" s="1">
-        <v>2.48</v>
+        <v>0</v>
       </c>
       <c r="F17" s="1">
         <v>1.81</v>
@@ -1053,10 +1124,14 @@
         <v>0.85</v>
       </c>
       <c r="H17" s="1">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>10.459999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1079,10 +1154,14 @@
         <v>4.3899999999999997</v>
       </c>
       <c r="H18" s="1">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1105,10 +1184,14 @@
         <v>2.76</v>
       </c>
       <c r="H19" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>11.44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1131,10 +1214,14 @@
         <v>2.78</v>
       </c>
       <c r="H20" s="1">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>14.61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1157,10 +1244,14 @@
         <v>2.25</v>
       </c>
       <c r="H21" s="1">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>13.26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1183,10 +1274,14 @@
         <v>1.24</v>
       </c>
       <c r="H22" s="1">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>12.76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1209,10 +1304,14 @@
         <v>3.7</v>
       </c>
       <c r="H23" s="1">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>13.45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1235,10 +1334,14 @@
         <v>2.68</v>
       </c>
       <c r="H24" s="1">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>12.45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1261,10 +1364,14 @@
         <v>0.98</v>
       </c>
       <c r="H25" s="1">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1287,10 +1394,14 @@
         <v>2.44</v>
       </c>
       <c r="H26" s="1">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>9.9400000000000013</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1313,10 +1424,14 @@
         <v>3.89</v>
       </c>
       <c r="H27" s="1">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1341,8 +1456,12 @@
       <c r="H28" s="1">
         <v>84</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>13.23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1365,10 +1484,14 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="H29" s="1">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>12.689999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1391,10 +1514,14 @@
         <v>1.95</v>
       </c>
       <c r="H30" s="1">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>12.689999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -1417,10 +1544,14 @@
         <v>1.26</v>
       </c>
       <c r="H31" s="1">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>12.33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -1443,10 +1574,14 @@
         <v>2.0099999999999998</v>
       </c>
       <c r="H32" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>12.34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -1469,10 +1604,14 @@
         <v>2.0699999999999998</v>
       </c>
       <c r="H33" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>11.77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1495,10 +1634,14 @@
         <v>4.72</v>
       </c>
       <c r="H34" s="1">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>14.39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -1512,7 +1655,7 @@
         <v>0.86</v>
       </c>
       <c r="E35" s="1">
-        <v>1.74</v>
+        <v>0</v>
       </c>
       <c r="F35" s="1">
         <v>2.5499999999999998</v>
@@ -1523,8 +1666,12 @@
       <c r="H35" s="1">
         <v>73</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>11.49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -1549,8 +1696,12 @@
       <c r="H36" s="1">
         <v>78</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -1564,7 +1715,7 @@
         <v>0.52</v>
       </c>
       <c r="E37" s="1">
-        <v>2.34</v>
+        <v>0</v>
       </c>
       <c r="F37" s="1">
         <v>1.54</v>
@@ -1574,6 +1725,10 @@
       </c>
       <c r="H37" s="1">
         <v>82</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>9.42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>